<commit_message>
day 16 part 1 done
</commit_message>
<xml_diff>
--- a/Day16/psudeo.xlsx
+++ b/Day16/psudeo.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day16/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{8B5CCECA-708E-0B4C-B953-40D8F16EB8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A73E37A4-FC90-0549-B0A9-3B6B522E7888}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{8B5CCECA-708E-0B4C-B953-40D8F16EB8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975FA563-C071-C947-9790-6BF251DAFFC2}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="1180" windowWidth="25680" windowHeight="17400" activeTab="1" xr2:uid="{405CFDC8-5423-8A42-8454-98F197F0DD4F}"/>
+    <workbookView xWindow="5660" yWindow="40" windowWidth="25680" windowHeight="17400" activeTab="2" xr2:uid="{405CFDC8-5423-8A42-8454-98F197F0DD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>version</t>
   </si>
@@ -187,12 +188,15 @@
   <si>
     <t>S</t>
   </si>
+  <si>
+    <t>1.0100000011001E+36</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,6 +211,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D4A1CA-18F8-6146-B7D2-44C91852FEDA}">
   <dimension ref="D7:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H23:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,4 +1275,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869759C1-FF87-DA4E-BDB6-761B7886E606}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="77.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>